<commit_message>
small fixes to date calculation adds some logging
</commit_message>
<xml_diff>
--- a/src/data/excel.xlsx
+++ b/src/data/excel.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11208"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10113"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dybapi/PycharmProjects/gfi-vue-gantt-elastic/src/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43A5F1C2-0176-E94A-BDF0-E6C41F095F20}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2524B88A-5E18-8940-96CE-94396ABE46E8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="35840" windowHeight="21200" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="35840" windowHeight="21200" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="teams" sheetId="6" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="91">
   <si>
     <t>ID</t>
   </si>
@@ -274,6 +274,36 @@
   </si>
   <si>
     <t>143087, 143088</t>
+  </si>
+  <si>
+    <t>Release Pipeline Support - Sprint 11.5 - Team Buzzard-Apes</t>
+  </si>
+  <si>
+    <t>Release Pipeline Support - Sprint 11.5 - Team Buzzard-Monkeys</t>
+  </si>
+  <si>
+    <t>Release Pipeline Support - Sprint 12.1 - Team Buzzard-Apes</t>
+  </si>
+  <si>
+    <t>Release Pipeline Support - Sprint 12.1 - Team Buzzard-Monkeys</t>
+  </si>
+  <si>
+    <t>Release Pipeline Support - Sprint 12.2 - Team Buzzard-Apes</t>
+  </si>
+  <si>
+    <t>Release Pipeline Support - Sprint 12.2- Team Buzzard-Monkeys</t>
+  </si>
+  <si>
+    <t>Release Pipeline Support - Sprint 12.3- Team Buzzard-Apes</t>
+  </si>
+  <si>
+    <t>Release Pipeline Support - Sprint 12.3 - Team Buzzard-Monkeys</t>
+  </si>
+  <si>
+    <t>Release Pipeline Support - Sprint 12.4 - Team Buzzard-Apes</t>
+  </si>
+  <si>
+    <t>Release Pipeline Support - Sprint 12.4 - Team Buzzard-Monkeys</t>
   </si>
 </sst>
 </file>
@@ -392,7 +422,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -405,6 +435,9 @@
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="14" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="27">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -775,8 +808,8 @@
   </sheetPr>
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -797,7 +830,7 @@
         <v>14</v>
       </c>
       <c r="B2">
-        <v>2</v>
+        <v>44</v>
       </c>
       <c r="C2" s="4">
         <v>43842</v>
@@ -860,10 +893,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:J27"/>
+  <dimension ref="A1:J37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="94" zoomScaleNormal="94" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1:J4"/>
+    <sheetView zoomScale="94" zoomScaleNormal="94" workbookViewId="0">
+      <selection activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1001,7 +1034,7 @@
         <v>43837</v>
       </c>
       <c r="G6">
-        <v>74</v>
+        <v>84</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
@@ -1041,7 +1074,7 @@
         <v>66</v>
       </c>
       <c r="E8" s="5">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="F8" s="8">
         <v>43837</v>
@@ -1084,15 +1117,8 @@
       <c r="E10" s="5">
         <v>2</v>
       </c>
-      <c r="F10" s="8">
-        <v>43844</v>
-      </c>
-      <c r="G10">
-        <v>45</v>
-      </c>
-      <c r="H10" s="5">
-        <v>50</v>
-      </c>
+      <c r="F10" s="8"/>
+      <c r="H10" s="5"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" s="5">
@@ -1201,7 +1227,7 @@
       </c>
       <c r="F16" s="8"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="5">
         <v>138624</v>
       </c>
@@ -1219,7 +1245,7 @@
       </c>
       <c r="F17" s="8"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="5">
         <v>139426</v>
       </c>
@@ -1237,7 +1263,7 @@
       </c>
       <c r="F18" s="8"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" s="5">
         <v>138472</v>
       </c>
@@ -1253,9 +1279,14 @@
       <c r="E19" s="5">
         <v>13</v>
       </c>
-      <c r="F19" s="5"/>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F19" s="4">
+        <v>43894</v>
+      </c>
+      <c r="G19">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" s="5">
         <v>139428</v>
       </c>
@@ -1273,7 +1304,7 @@
       </c>
       <c r="F20" s="5"/>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" s="5">
         <v>140663</v>
       </c>
@@ -1291,7 +1322,7 @@
       </c>
       <c r="F21" s="5"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" s="5">
         <v>142434</v>
       </c>
@@ -1309,7 +1340,7 @@
       </c>
       <c r="F22" s="5"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" s="5">
         <v>135450</v>
       </c>
@@ -1327,7 +1358,7 @@
       </c>
       <c r="F23" s="5"/>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" s="5">
         <v>138621</v>
       </c>
@@ -1344,7 +1375,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" s="5">
         <v>142435</v>
       </c>
@@ -1361,7 +1392,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" s="5">
         <v>142436</v>
       </c>
@@ -1378,7 +1409,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" s="5">
         <v>142439</v>
       </c>
@@ -1393,6 +1424,236 @@
       </c>
       <c r="E27" s="5">
         <v>5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A28" s="5">
+        <v>200001</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D28" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="E28" s="5">
+        <v>8</v>
+      </c>
+      <c r="F28" s="8">
+        <v>43851</v>
+      </c>
+      <c r="G28">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A29" s="5">
+        <v>200002</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="C29" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D29" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="E29" s="5">
+        <v>7</v>
+      </c>
+      <c r="F29" s="8">
+        <v>43851</v>
+      </c>
+      <c r="G29">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A30" s="5">
+        <v>200003</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="C30" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D30" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="E30" s="5">
+        <v>8</v>
+      </c>
+      <c r="F30" s="10">
+        <v>43866</v>
+      </c>
+      <c r="G30">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A31" s="5">
+        <v>200004</v>
+      </c>
+      <c r="B31" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="C31" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D31" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="E31" s="5">
+        <v>7</v>
+      </c>
+      <c r="F31" s="10">
+        <v>43866</v>
+      </c>
+      <c r="G31">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A32" s="5">
+        <v>200005</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="C32" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D32" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="E32" s="5">
+        <v>8</v>
+      </c>
+      <c r="F32" s="4">
+        <v>43880</v>
+      </c>
+      <c r="G32">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A33" s="5">
+        <v>200006</v>
+      </c>
+      <c r="B33" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="C33" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D33" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="E33" s="5">
+        <v>7</v>
+      </c>
+      <c r="F33" s="4">
+        <v>43880</v>
+      </c>
+      <c r="G33">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A34" s="5">
+        <v>200007</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="C34" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D34" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="E34" s="5">
+        <v>8</v>
+      </c>
+      <c r="F34" s="4">
+        <v>43894</v>
+      </c>
+      <c r="G34">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A35" s="5">
+        <v>200008</v>
+      </c>
+      <c r="B35" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="C35" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D35" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="E35" s="5">
+        <v>7</v>
+      </c>
+      <c r="F35" s="4">
+        <v>43894</v>
+      </c>
+      <c r="G35">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A36" s="5">
+        <v>200009</v>
+      </c>
+      <c r="B36" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="C36" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D36" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="E36" s="5">
+        <v>8</v>
+      </c>
+      <c r="F36" s="4">
+        <v>43908</v>
+      </c>
+      <c r="G36">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A37" s="5">
+        <v>200010</v>
+      </c>
+      <c r="B37" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="C37" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D37" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="E37" s="5">
+        <v>7</v>
+      </c>
+      <c r="F37" s="4">
+        <v>43908</v>
+      </c>
+      <c r="G37">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adds systeam lmf fixes common team issue
</commit_message>
<xml_diff>
--- a/src/data/excel.xlsx
+++ b/src/data/excel.xlsx
@@ -8,18 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dybapi/PycharmProjects/gfi-vue-gantt-elastic/src/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2524B88A-5E18-8940-96CE-94396ABE46E8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C41E394C-E453-E94C-8823-C810E7F18691}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="35840" windowHeight="21200" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="35840" windowHeight="21200" tabRatio="500" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="teams" sheetId="6" r:id="rId1"/>
-    <sheet name="infrastructure" sheetId="1" r:id="rId2"/>
-    <sheet name="bi" sheetId="2" r:id="rId3"/>
-    <sheet name="sm" sheetId="3" r:id="rId4"/>
-    <sheet name="integration" sheetId="4" r:id="rId5"/>
-    <sheet name="epsui" sheetId="5" r:id="rId6"/>
-    <sheet name="Sheet1" sheetId="7" r:id="rId7"/>
+    <sheet name="systeam" sheetId="7" r:id="rId2"/>
+    <sheet name="infrastructure" sheetId="1" r:id="rId3"/>
+    <sheet name="bi" sheetId="2" r:id="rId4"/>
+    <sheet name="sm" sheetId="3" r:id="rId5"/>
+    <sheet name="integration" sheetId="4" r:id="rId6"/>
+    <sheet name="epsui" sheetId="5" r:id="rId7"/>
+    <sheet name="lmf" sheetId="9" r:id="rId8"/>
+    <sheet name="Sheet1" sheetId="8" r:id="rId9"/>
   </sheets>
   <calcPr calcId="140000"/>
   <extLst>
@@ -31,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="99">
   <si>
     <t>ID</t>
   </si>
@@ -304,6 +306,30 @@
   </si>
   <si>
     <t>Release Pipeline Support - Sprint 12.4 - Team Buzzard-Monkeys</t>
+  </si>
+  <si>
+    <t>systeam</t>
+  </si>
+  <si>
+    <t>sys1</t>
+  </si>
+  <si>
+    <t>sys2</t>
+  </si>
+  <si>
+    <t>sys3</t>
+  </si>
+  <si>
+    <t>lmf</t>
+  </si>
+  <si>
+    <t>lmf 1</t>
+  </si>
+  <si>
+    <t>lmf 2</t>
+  </si>
+  <si>
+    <t>lmf 3</t>
   </si>
 </sst>
 </file>
@@ -806,10 +832,10 @@
   <sheetPr>
     <tabColor rgb="FFFF0000"/>
   </sheetPr>
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -878,6 +904,28 @@
       </c>
       <c r="C6" s="4">
         <v>43750</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>91</v>
+      </c>
+      <c r="B7">
+        <v>28</v>
+      </c>
+      <c r="C7" s="4">
+        <v>43850</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>95</v>
+      </c>
+      <c r="B8">
+        <v>10</v>
+      </c>
+      <c r="C8" s="4">
+        <v>43850</v>
       </c>
     </row>
   </sheetData>
@@ -892,6 +940,112 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09F35A67-FEEB-7540-BF66-07A7A9D7E75B}">
+  <dimension ref="A1:H4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B41" sqref="B40:B41"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="8.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="84.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="13.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="G1" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="H1" s="9" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>123121</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="2">
+        <v>2</v>
+      </c>
+      <c r="H2" s="2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>123124</v>
+      </c>
+      <c r="B3" t="s">
+        <v>93</v>
+      </c>
+      <c r="C3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3">
+        <v>8</v>
+      </c>
+      <c r="H3">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>123125</v>
+      </c>
+      <c r="B4" t="s">
+        <v>94</v>
+      </c>
+      <c r="C4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4">
+        <v>20</v>
+      </c>
+      <c r="H4">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:J37"/>
   <sheetViews>
@@ -1667,7 +1821,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:H4"/>
   <sheetViews>
@@ -1769,7 +1923,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:H4"/>
   <sheetViews>
@@ -1871,12 +2025,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="A2" sqref="A2:E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1973,12 +2127,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="D41" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2075,15 +2229,20 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09F35A67-FEEB-7540-BF66-07A7A9D7E75B}">
-  <dimension ref="A1:H1"/>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{898DCDDC-731F-674A-91E4-10BD9DC4A347}">
+  <dimension ref="A1:H4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="8.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="84.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="13.33203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
@@ -2111,6 +2270,103 @@
         <v>36</v>
       </c>
     </row>
+    <row r="2" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>30331</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>30332</v>
+      </c>
+      <c r="B3" t="s">
+        <v>97</v>
+      </c>
+      <c r="C3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>30333</v>
+      </c>
+      <c r="B4" t="s">
+        <v>98</v>
+      </c>
+      <c r="C4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03816021-39E8-DB49-A703-71D18FF3E9D9}">
+  <dimension ref="A1:H1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="8.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="84.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="13.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="G1" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="H1" s="9" t="s">
+        <v>36</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>